<commit_message>
cap nhat quy trinh
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>URL</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>off_2/9_to</t>
+  </si>
+  <si>
+    <t>admin_vinhtrinh</t>
+  </si>
+  <si>
+    <t>Unitech@</t>
   </si>
 </sst>
 </file>
@@ -535,12 +541,12 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.6328125" customWidth="1"/>
+    <col min="1" max="1" width="36.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
@@ -638,7 +644,15 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C3" s="2"/>
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="12"/>
@@ -651,8 +665,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>